<commit_message>
external zone setting parameter with not setting value case dealt
</commit_message>
<xml_diff>
--- a/protection_zones_external_parameters.xlsx
+++ b/protection_zones_external_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Masterthesis\IEET\pycharmtest\backup_code_masterthesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50174E07-D247-4C6E-8D97-44DE154CF805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE386F93-2381-42E7-818D-A551E9F6E9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{6DAA9567-C7A5-48E3-811D-4B5326483F6A}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{6DAA9567-C7A5-48E3-811D-4B5326483F6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -529,24 +529,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AADA4ACB-3BF2-4149-BBE1-9994162843FE}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:N9"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" customWidth="1"/>
-    <col min="3" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.88671875" customWidth="1"/>
-    <col min="13" max="14" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="4" width="12.78515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.78515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.78515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.85546875" customWidth="1"/>
+    <col min="13" max="14" width="12.78515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -590,7 +590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -634,7 +634,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -678,7 +678,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -722,7 +722,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -766,7 +766,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -810,7 +810,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -854,7 +854,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -898,7 +898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -942,7 +942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -986,7 +986,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>

</xml_diff>